<commit_message>
new mbr code,+ debug
</commit_message>
<xml_diff>
--- a/analysis/infos/HCS_MBR_Code_Details.xlsx
+++ b/analysis/infos/HCS_MBR_Code_Details.xlsx
@@ -1,19 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cogneuro\Desktop\HCS_analysis\analysis\infos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="MBR File Format" sheetId="1" r:id="rId4"/>
-    <sheet name="Short Behavior Codes" sheetId="2" r:id="rId5"/>
-    <sheet name="Long Behavior Codes" sheetId="3" r:id="rId6"/>
+    <sheet name="MBR File Format" sheetId="1" r:id="rId1"/>
+    <sheet name="Short Behavior Codes" sheetId="2" r:id="rId2"/>
+    <sheet name="Long Behavior Codes" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="117">
   <si>
     <t>MBR File Format:</t>
   </si>
@@ -370,27 +378,17 @@
   <si>
     <t>Behavior code</t>
   </si>
+  <si>
+    <t>Arousal</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -400,7 +398,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -597,157 +595,134 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+  <cellXfs count="50">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -757,29 +732,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffdd0806"/>
-      <rgbColor rgb="ffccffcc"/>
-      <rgbColor rgb="ffff99cc"/>
-      <rgbColor rgb="ffffcc00"/>
-      <rgbColor rgb="fffcf305"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFDD0806"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFCF305"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -911,7 +942,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -987,7 +1018,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1006,7 +1037,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1036,7 +1067,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1062,7 +1093,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1088,7 +1119,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1114,7 +1145,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1140,7 +1171,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1166,7 +1197,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1192,7 +1223,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1218,7 +1249,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1244,7 +1275,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1257,9 +1288,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1274,7 +1311,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="38000"/>
             </a:srgbClr>
@@ -1282,7 +1319,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1301,7 +1338,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1327,7 +1364,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1353,7 +1390,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1379,7 +1416,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1405,7 +1442,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1431,7 +1468,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1457,7 +1494,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1483,7 +1520,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1509,7 +1546,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1535,7 +1572,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1548,9 +1585,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1564,7 +1607,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1583,7 +1626,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1613,7 +1656,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1639,7 +1682,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1665,7 +1708,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1691,7 +1734,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1717,7 +1760,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1743,7 +1786,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1769,7 +1812,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1795,7 +1838,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1821,7 +1864,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1834,34 +1877,41 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV18"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.8516" style="1" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="1" customWidth="1"/>
+    <col min="6" max="256" width="8.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
@@ -1869,8 +1919,8 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="4">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3"/>
@@ -1878,8 +1928,8 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="4">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3"/>
@@ -1887,8 +1937,8 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="5">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3"/>
@@ -1896,8 +1946,8 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="5">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3"/>
@@ -1905,8 +1955,8 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="4">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="3"/>
@@ -1914,8 +1964,8 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="4">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3"/>
@@ -1923,22 +1973,22 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" t="s" s="2">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="3"/>
@@ -1946,8 +1996,8 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" ht="15" customHeight="1">
-      <c r="A11" t="s" s="2">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="3"/>
@@ -1955,8 +2005,8 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" ht="15" customHeight="1">
-      <c r="A12" t="s" s="2">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="3"/>
@@ -1964,8 +2014,8 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" ht="15" customHeight="1">
-      <c r="A13" t="s" s="2">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="3"/>
@@ -1973,8 +2023,8 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" ht="15" customHeight="1">
-      <c r="A14" t="s" s="2">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="3"/>
@@ -1982,8 +2032,8 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" ht="15" customHeight="1">
-      <c r="A15" t="s" s="2">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="3"/>
@@ -1991,8 +2041,8 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" ht="15" customHeight="1">
-      <c r="A16" t="s" s="2">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="3"/>
@@ -2000,14 +2050,14 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" ht="15" customHeight="1">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" ht="15" customHeight="1">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2016,7 +2066,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2024,23 +2074,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV61"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.3516" style="7" customWidth="1"/>
-    <col min="2" max="2" width="23.3516" style="7" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="7" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="7" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="7" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="7" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="7" customWidth="1"/>
+    <col min="3" max="256" width="8.85546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="8">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="3"/>
@@ -2048,712 +2097,712 @@
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="8">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s" s="8">
+      <c r="B2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s" s="10">
+      <c r="C2" s="10" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>0</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s" s="10">
+      <c r="C3" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>1</v>
       </c>
-      <c r="B4" t="s" s="2">
+      <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s" s="10">
+      <c r="C4" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>2</v>
       </c>
-      <c r="B5" t="s" s="2">
+      <c r="B5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s" s="10">
+      <c r="C5" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>3</v>
       </c>
-      <c r="B6" t="s" s="2">
+      <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s" s="10">
+      <c r="C6" s="10" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>4</v>
       </c>
-      <c r="B7" t="s" s="2">
+      <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s" s="10">
+      <c r="C7" s="10" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>5</v>
       </c>
-      <c r="B8" t="s" s="2">
+      <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C8" t="s" s="10">
+      <c r="C8" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>6</v>
       </c>
-      <c r="B9" t="s" s="2">
+      <c r="B9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s" s="10">
+      <c r="C9" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>7</v>
       </c>
-      <c r="B10" t="s" s="2">
+      <c r="B10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s" s="10">
+      <c r="C10" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" ht="15" customHeight="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>8</v>
       </c>
-      <c r="B11" t="s" s="2">
+      <c r="B11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s" s="10">
+      <c r="C11" s="10" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>9</v>
       </c>
-      <c r="B12" t="s" s="2">
+      <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s" s="10">
+      <c r="C12" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
     </row>
-    <row r="13" ht="15" customHeight="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>10</v>
       </c>
-      <c r="B13" t="s" s="2">
+      <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C13" t="s" s="10">
+      <c r="C13" s="10" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
     </row>
-    <row r="14" ht="15" customHeight="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>11</v>
       </c>
-      <c r="B14" t="s" s="2">
+      <c r="B14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C14" t="s" s="10">
+      <c r="C14" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
     </row>
-    <row r="15" ht="15" customHeight="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>12</v>
       </c>
-      <c r="B15" t="s" s="2">
+      <c r="B15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C15" t="s" s="10">
+      <c r="C15" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>13</v>
       </c>
-      <c r="B16" t="s" s="2">
+      <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C16" t="s" s="10">
+      <c r="C16" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
     </row>
-    <row r="17" ht="15" customHeight="1">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>14</v>
       </c>
-      <c r="B17" t="s" s="2">
+      <c r="B17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C17" t="s" s="10">
+      <c r="C17" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
     </row>
-    <row r="18" ht="15" customHeight="1">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>15</v>
       </c>
-      <c r="B18" t="s" s="2">
+      <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C18" t="s" s="10">
+      <c r="C18" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" ht="15" customHeight="1">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>16</v>
       </c>
-      <c r="B19" t="s" s="2">
+      <c r="B19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C19" t="s" s="10">
+      <c r="C19" s="10" t="s">
         <v>47</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" ht="15" customHeight="1">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>17</v>
       </c>
-      <c r="B20" t="s" s="2">
+      <c r="B20" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C20" t="s" s="10">
+      <c r="C20" s="10" t="s">
         <v>49</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
     </row>
-    <row r="21" ht="15" customHeight="1">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>18</v>
       </c>
-      <c r="B21" t="s" s="2">
+      <c r="B21" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C21" t="s" s="10">
+      <c r="C21" s="10" t="s">
         <v>49</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
     </row>
-    <row r="22" ht="15" customHeight="1">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>19</v>
       </c>
-      <c r="B22" t="s" s="2">
+      <c r="B22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C22" t="s" s="10">
+      <c r="C22" s="10" t="s">
         <v>51</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
     </row>
-    <row r="23" ht="15" customHeight="1">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>20</v>
       </c>
-      <c r="B23" t="s" s="2">
+      <c r="B23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C23" t="s" s="10">
+      <c r="C23" s="10" t="s">
         <v>53</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
     </row>
-    <row r="24" ht="15" customHeight="1">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>21</v>
       </c>
-      <c r="B24" t="s" s="2">
+      <c r="B24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C24" t="s" s="10">
+      <c r="C24" s="10" t="s">
         <v>55</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
     </row>
-    <row r="25" ht="15" customHeight="1">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>22</v>
       </c>
-      <c r="B25" t="s" s="2">
+      <c r="B25" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C25" t="s" s="10">
+      <c r="C25" s="10" t="s">
         <v>57</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
     </row>
-    <row r="26" ht="15" customHeight="1">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>23</v>
       </c>
-      <c r="B26" t="s" s="2">
+      <c r="B26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C26" t="s" s="10">
+      <c r="C26" s="10" t="s">
         <v>59</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
     </row>
-    <row r="27" ht="15" customHeight="1">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>24</v>
       </c>
-      <c r="B27" t="s" s="2">
+      <c r="B27" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C27" t="s" s="10">
+      <c r="C27" s="10" t="s">
         <v>61</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
     </row>
-    <row r="28" ht="15" customHeight="1">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>25</v>
       </c>
-      <c r="B28" t="s" s="2">
+      <c r="B28" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C28" t="s" s="10">
+      <c r="C28" s="10" t="s">
         <v>63</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
     </row>
-    <row r="29" ht="15" customHeight="1">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>26</v>
       </c>
-      <c r="B29" t="s" s="2">
+      <c r="B29" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C29" t="s" s="10">
+      <c r="C29" s="10" t="s">
         <v>65</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" ht="15" customHeight="1">
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>27</v>
       </c>
-      <c r="B30" t="s" s="2">
+      <c r="B30" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C30" t="s" s="10">
+      <c r="C30" s="10" t="s">
         <v>67</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
     </row>
-    <row r="31" ht="15" customHeight="1">
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>28</v>
       </c>
-      <c r="B31" t="s" s="2">
+      <c r="B31" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C31" t="s" s="10">
+      <c r="C31" s="10" t="s">
         <v>69</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" ht="15" customHeight="1">
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>29</v>
       </c>
-      <c r="B32" t="s" s="2">
+      <c r="B32" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C32" t="s" s="10">
+      <c r="C32" s="10" t="s">
         <v>71</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
     </row>
-    <row r="33" ht="15" customHeight="1">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>30</v>
       </c>
-      <c r="B33" t="s" s="2">
+      <c r="B33" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C33" t="s" s="10">
+      <c r="C33" s="10" t="s">
         <v>73</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
     </row>
-    <row r="34" ht="15" customHeight="1">
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>31</v>
       </c>
-      <c r="B34" t="s" s="2">
+      <c r="B34" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C34" t="s" s="10">
-        <v>73</v>
+      <c r="C34" s="10" t="s">
+        <v>116</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
     </row>
-    <row r="35" ht="15" customHeight="1">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>32</v>
       </c>
-      <c r="B35" t="s" s="2">
+      <c r="B35" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C35" t="s" s="10">
+      <c r="C35" s="10" t="s">
         <v>76</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
     </row>
-    <row r="36" ht="15" customHeight="1">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <v>33</v>
       </c>
-      <c r="B36" t="s" s="2">
+      <c r="B36" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C36" t="s" s="10">
+      <c r="C36" s="10" t="s">
         <v>78</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
     </row>
-    <row r="37" ht="15" customHeight="1">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
         <v>34</v>
       </c>
-      <c r="B37" t="s" s="2">
+      <c r="B37" s="2" t="s">
         <v>79</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
     </row>
-    <row r="38" ht="15" customHeight="1">
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>35</v>
       </c>
-      <c r="B38" t="s" s="2">
+      <c r="B38" s="2" t="s">
         <v>80</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
     </row>
-    <row r="39" ht="15" customHeight="1">
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
         <v>36</v>
       </c>
-      <c r="B39" t="s" s="2">
+      <c r="B39" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C39" t="s" s="10">
+      <c r="C39" s="10" t="s">
         <v>82</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
     </row>
-    <row r="40" ht="15" customHeight="1">
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11">
         <v>37</v>
       </c>
-      <c r="B40" t="s" s="2">
+      <c r="B40" s="2" t="s">
         <v>83</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
     </row>
-    <row r="41" ht="15" customHeight="1">
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
         <v>38</v>
       </c>
-      <c r="B41" t="s" s="2">
+      <c r="B41" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C41" t="s" s="10">
+      <c r="C41" s="10" t="s">
         <v>85</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
     </row>
-    <row r="42" ht="15" customHeight="1">
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11">
         <v>39</v>
       </c>
-      <c r="B42" t="s" s="2">
+      <c r="B42" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C42" t="s" s="10">
+      <c r="C42" s="10" t="s">
         <v>87</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
     </row>
-    <row r="43" ht="15" customHeight="1">
+    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
         <v>40</v>
       </c>
-      <c r="B43" t="s" s="2">
+      <c r="B43" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C43" t="s" s="10">
+      <c r="C43" s="10" t="s">
         <v>89</v>
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
     </row>
-    <row r="44" ht="15" customHeight="1">
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11">
         <v>41</v>
       </c>
-      <c r="B44" t="s" s="2">
+      <c r="B44" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C44" t="s" s="10">
+      <c r="C44" s="10" t="s">
         <v>91</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
     </row>
-    <row r="45" ht="15" customHeight="1">
+    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
         <v>42</v>
       </c>
-      <c r="B45" t="s" s="2">
+      <c r="B45" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C45" t="s" s="10">
+      <c r="C45" s="10" t="s">
         <v>93</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
     </row>
-    <row r="46" ht="15" customHeight="1">
+    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
         <v>43</v>
       </c>
-      <c r="B46" t="s" s="2">
+      <c r="B46" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C46" t="s" s="10">
+      <c r="C46" s="10" t="s">
         <v>95</v>
       </c>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
     </row>
-    <row r="47" ht="15" customHeight="1">
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
         <v>44</v>
       </c>
-      <c r="B47" t="s" s="2">
+      <c r="B47" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
     </row>
-    <row r="48" ht="15" customHeight="1">
+    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
         <v>45</v>
       </c>
-      <c r="B48" t="s" s="2">
+      <c r="B48" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C48" t="s" s="10">
+      <c r="C48" s="10" t="s">
         <v>98</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
     </row>
-    <row r="49" ht="15" customHeight="1">
+    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
         <v>46</v>
       </c>
-      <c r="B49" t="s" s="2">
+      <c r="B49" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C49" t="s" s="10">
+      <c r="C49" s="10" t="s">
         <v>100</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
     </row>
-    <row r="50" ht="15" customHeight="1">
+    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <v>47</v>
       </c>
-      <c r="B50" t="s" s="2">
+      <c r="B50" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C50" t="s" s="10">
+      <c r="C50" s="10" t="s">
         <v>102</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
     </row>
-    <row r="51" ht="15" customHeight="1">
+    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
         <v>48</v>
       </c>
-      <c r="B51" t="s" s="2">
+      <c r="B51" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C51" t="s" s="10">
+      <c r="C51" s="10" t="s">
         <v>104</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
     </row>
-    <row r="52" ht="15" customHeight="1">
+    <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
     </row>
-    <row r="53" ht="15" customHeight="1">
+    <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
     </row>
-    <row r="54" ht="15" customHeight="1">
+    <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
     </row>
-    <row r="55" ht="15" customHeight="1">
+    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
     </row>
-    <row r="56" ht="15" customHeight="1">
+    <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
     </row>
-    <row r="57" ht="15" customHeight="1">
+    <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
       <c r="B57" s="3"/>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
     </row>
-    <row r="58" ht="15" customHeight="1">
+    <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
       <c r="B58" s="3"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
     </row>
-    <row r="59" ht="15" customHeight="1">
+    <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
       <c r="B59" s="3"/>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
     </row>
-    <row r="60" ht="15" customHeight="1">
+    <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
       <c r="B60" s="3"/>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
     </row>
-    <row r="61" ht="15" customHeight="1">
+    <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="3"/>
       <c r="C61" s="9"/>
@@ -2762,7 +2811,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2770,187 +2819,186 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6719" style="14" customWidth="1"/>
-    <col min="2" max="2" width="14.8516" style="14" customWidth="1"/>
-    <col min="3" max="3" width="24.6719" style="14" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="14" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="14" customWidth="1"/>
-    <col min="6" max="6" width="13.5" style="14" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="14" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="14" customWidth="1"/>
+    <col min="5" max="6" width="13.42578125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="14" customWidth="1"/>
     <col min="8" max="8" width="11" style="14" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="14" customWidth="1"/>
-    <col min="10" max="256" width="8.85156" style="14" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="14" customWidth="1"/>
+    <col min="10" max="256" width="8.85546875" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="15">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="16">
+      <c r="B1" s="15">
         <v>1</v>
       </c>
-      <c r="C1" s="17">
+      <c r="C1" s="16">
         <v>2</v>
       </c>
-      <c r="D1" s="18">
+      <c r="D1" s="17">
         <v>3</v>
       </c>
-      <c r="E1" s="18">
+      <c r="E1" s="17">
         <v>4</v>
       </c>
-      <c r="F1" s="18">
+      <c r="F1" s="17">
         <v>5</v>
       </c>
-      <c r="G1" s="19">
+      <c r="G1" s="18">
         <v>6</v>
       </c>
-      <c r="H1" s="19">
+      <c r="H1" s="18">
         <v>7</v>
       </c>
-      <c r="I1" s="20">
+      <c r="I1" s="19">
         <v>8</v>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="21"/>
-      <c r="B2" t="s" s="22">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="49"/>
+      <c r="B2" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="C2" t="s" s="23">
+      <c r="C2" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="D2" t="s" s="24">
+      <c r="D2" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="E2" t="s" s="24">
+      <c r="E2" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="F2" t="s" s="24">
+      <c r="F2" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="G2" t="s" s="25">
+      <c r="G2" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="H2" t="s" s="25">
+      <c r="H2" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I2" t="s" s="26">
+      <c r="I2" s="24" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" ht="39" customHeight="1">
-      <c r="A3" t="s" s="27">
+    <row r="3" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="B3" t="s" s="28">
+      <c r="B3" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-    </row>
-    <row r="4" ht="59.25" customHeight="1">
-      <c r="A4" t="s" s="31">
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+    </row>
+    <row r="4" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" t="s" s="33">
+      <c r="B4" s="30"/>
+      <c r="C4" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="37">
+      <c r="D4" s="32"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="39"/>
-      <c r="D5" t="s" s="24">
+      <c r="B5" s="35"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="E5" t="s" s="24">
+      <c r="E5" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="F5" t="s" s="24">
+      <c r="F5" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="G5" s="38"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-    </row>
-    <row r="6" ht="65.25" customHeight="1">
+      <c r="G5" s="35"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+    </row>
+    <row r="6" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="40"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="41"/>
-      <c r="D6" t="s" s="42">
+      <c r="B6" s="35"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="44">
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="39"/>
-      <c r="G7" t="s" s="25">
+      <c r="B7" s="35"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="H7" t="s" s="25">
+      <c r="H7" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="I7" t="s" s="26">
+      <c r="I7" s="24" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="45"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="41"/>
-      <c r="G8" t="s" s="25">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="42"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="H8" s="46"/>
-      <c r="I8" s="47"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="48"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="45"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="38"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2970,7 +3018,7 @@
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <pageSetup orientation="landscape"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>